<commit_message>
swapped ADC DCLK pins to match pass Anurag's test implementation
</commit_message>
<xml_diff>
--- a/hardware/Graviton SDRAM pin assignments.xlsx
+++ b/hardware/Graviton SDRAM pin assignments.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="17985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="17985" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SDRAM" sheetId="1" r:id="rId1"/>
+    <sheet name="ADC" sheetId="2" r:id="rId2"/>
+    <sheet name="DAC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="265">
   <si>
     <t>DDR Pin</t>
   </si>
@@ -705,6 +707,120 @@
   </si>
   <si>
     <t>AJ31</t>
+  </si>
+  <si>
+    <t>ADC-D0_P</t>
+  </si>
+  <si>
+    <t>ADC-D0_N</t>
+  </si>
+  <si>
+    <t>ADC-D1_P</t>
+  </si>
+  <si>
+    <t>ADC-D1_N</t>
+  </si>
+  <si>
+    <t>ADC-D2_P</t>
+  </si>
+  <si>
+    <t>ADC-D2_N</t>
+  </si>
+  <si>
+    <t>ADC-D3_P</t>
+  </si>
+  <si>
+    <t>ADC-D3_N</t>
+  </si>
+  <si>
+    <t>ADC-D4_P</t>
+  </si>
+  <si>
+    <t>ADC-D4_N</t>
+  </si>
+  <si>
+    <t>ADC-D5_P</t>
+  </si>
+  <si>
+    <t>ADC-D5_N</t>
+  </si>
+  <si>
+    <t>ADC-D6_P</t>
+  </si>
+  <si>
+    <t>ADC-D6_N</t>
+  </si>
+  <si>
+    <t>ADC-D7_P</t>
+  </si>
+  <si>
+    <t>ADC-D7_N</t>
+  </si>
+  <si>
+    <t>ADC-D8_P</t>
+  </si>
+  <si>
+    <t>ADC-D8_N</t>
+  </si>
+  <si>
+    <t>ADC-D9_P</t>
+  </si>
+  <si>
+    <t>ADC-D9_N</t>
+  </si>
+  <si>
+    <t>ADC-D10_P</t>
+  </si>
+  <si>
+    <t>ADC-D10_N</t>
+  </si>
+  <si>
+    <t>ADC-D11_P</t>
+  </si>
+  <si>
+    <t>ADC-D11_N</t>
+  </si>
+  <si>
+    <t>ADC-D12_P</t>
+  </si>
+  <si>
+    <t>ADC-D12_N</t>
+  </si>
+  <si>
+    <t>ADC-D13_P</t>
+  </si>
+  <si>
+    <t>ADC-D13_N</t>
+  </si>
+  <si>
+    <t>ADC-D14_P</t>
+  </si>
+  <si>
+    <t>ADC-D14_N</t>
+  </si>
+  <si>
+    <t>ADC-D15_P</t>
+  </si>
+  <si>
+    <t>ADC-D15_N</t>
+  </si>
+  <si>
+    <t>ADC-DCLK_P</t>
+  </si>
+  <si>
+    <t>ADC-DCLK_N</t>
+  </si>
+  <si>
+    <t>G1-DQ1</t>
+  </si>
+  <si>
+    <t>G1-DQ4</t>
+  </si>
+  <si>
+    <t>P30</t>
+  </si>
+  <si>
+    <t>N32</t>
   </si>
 </sst>
 </file>
@@ -1033,13 +1149,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
@@ -2107,4 +2223,544 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>245</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>259</v>
+      </c>
+      <c r="C34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>260</v>
+      </c>
+      <c r="C35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>